<commit_message>
user input sheet 1 compleet (I think)
</commit_message>
<xml_diff>
--- a/input/user_input.xlsx
+++ b/input/user_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B71D54C-9331-4064-B4DA-68C81DB6ADEA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0197FA3B-BC8D-4916-9514-B41CBB42CFD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>analysis</t>
   </si>
@@ -269,6 +269,12 @@
   </si>
   <si>
     <t>file names where information on infrastructure usage is stored: the Average Annual Daily Traffic and costs per vehicle type</t>
+  </si>
+  <si>
+    <t>hazard_unique_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name of the unique ID column if the hazard data is a shapefile and the data can be joined with the network by ID </t>
   </si>
 </sst>
 </file>
@@ -734,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,17 +761,17 @@
     <col min="11" max="11" width="13.44140625" customWidth="1"/>
     <col min="12" max="12" width="29" customWidth="1"/>
     <col min="13" max="13" width="18.44140625" customWidth="1"/>
-    <col min="14" max="14" width="22.21875" customWidth="1"/>
-    <col min="15" max="15" width="21.77734375" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
-    <col min="17" max="17" width="16.88671875" customWidth="1"/>
-    <col min="18" max="18" width="12" customWidth="1"/>
-    <col min="19" max="19" width="17.88671875" customWidth="1"/>
-    <col min="20" max="20" width="26.33203125" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="14" max="15" width="22.21875" customWidth="1"/>
+    <col min="16" max="16" width="21.77734375" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.88671875" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="17.88671875" customWidth="1"/>
+    <col min="21" max="21" width="26.33203125" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -809,28 +815,31 @@
         <v>57</v>
       </c>
       <c r="O1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="16" t="s">
+      <c r="V1" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
@@ -864,8 +873,9 @@
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V2" s="5"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -887,8 +897,9 @@
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3" s="5"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -910,8 +921,9 @@
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -933,6 +945,7 @@
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -980,7 +993,7 @@
           <x14:formula1>
             <xm:f>options!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576</xm:sqref>
+          <xm:sqref>Q2:Q1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -993,7 +1006,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8FA5B4-8351-441E-BC93-E5502E84268F}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,18 +1176,18 @@
     <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.21875" customWidth="1"/>
     <col min="13" max="13" width="22.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="16.77734375" customWidth="1"/>
-    <col min="16" max="16" width="19.44140625" customWidth="1"/>
-    <col min="17" max="17" width="17.109375" customWidth="1"/>
-    <col min="18" max="18" width="19.44140625" customWidth="1"/>
-    <col min="19" max="19" width="19.33203125" customWidth="1"/>
-    <col min="20" max="20" width="17.21875" customWidth="1"/>
-    <col min="21" max="21" width="16.77734375" customWidth="1"/>
-    <col min="22" max="22" width="16.33203125" customWidth="1"/>
+    <col min="14" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="16.77734375" customWidth="1"/>
+    <col min="17" max="17" width="19.44140625" customWidth="1"/>
+    <col min="18" max="18" width="17.109375" customWidth="1"/>
+    <col min="19" max="19" width="19.44140625" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" customWidth="1"/>
+    <col min="21" max="21" width="17.21875" customWidth="1"/>
+    <col min="22" max="22" width="16.77734375" customWidth="1"/>
+    <col min="23" max="23" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1218,31 +1231,34 @@
         <v>33</v>
       </c>
       <c r="O1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="U1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="W1" s="17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
@@ -1281,30 +1297,33 @@
       <c r="N2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12" t="s">
+      <c r="O2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="T2" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="U2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="V2" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="W2" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
Last commit of sprint October 2020: criticality full range single link and multilink analyses work (not yet the O/D). More testing required!!
</commit_message>
<xml_diff>
--- a/input/user_input.xlsx
+++ b/input/user_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0197FA3B-BC8D-4916-9514-B41CBB42CFD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62797163-B5A2-430A-89AC-654716DB8DB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated input excel and explanation
</commit_message>
<xml_diff>
--- a/input/user_input.xlsx
+++ b/input/user_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1D4D4B-DC61-43C2-8DDA-CCAAEDD00D82}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC3D29F-9A70-40B8-91EB-B35EFCA63F54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t>analysis</t>
   </si>
@@ -152,23 +152,6 @@
     <t>Name that you want to give to the analysis (output files will start with this name)</t>
   </si>
   <si>
-    <t>When choosing network_source based on OSM. Provide name of shapefile with region for OSM input &lt;rel path is in config file)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">When chosen voor network based on shapefile indicate shapefile for analysis - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>consider removing and linking to config file?</t>
-    </r>
-  </si>
-  <si>
     <t>In case a Unique ID exists, indicate here the column of the shapefile. If you want the tool to create a new one, leave empty</t>
   </si>
   <si>
@@ -275,13 +258,25 @@
   </si>
   <si>
     <t xml:space="preserve">name of the unique ID column if the hazard data is a shapefile and the data can be joined with the network by ID </t>
+  </si>
+  <si>
+    <t>path_to_pbf</t>
+  </si>
+  <si>
+    <t>When choosing network_source based on OSM online. Provide name of shapefile with region for OSM input &lt;rel path is in config file&gt;. No extension needed.</t>
+  </si>
+  <si>
+    <t>When choosing network_source based on OSM dump. Provide name of *.pbf dump. No extension needed.</t>
+  </si>
+  <si>
+    <t>When choosing for network based on shapefile indicate shapefile for analysis.  Provide name of shapefile. No extension needed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,12 +313,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -727,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,27 +728,27 @@
     <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
-    <col min="12" max="12" width="29" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" customWidth="1"/>
-    <col min="14" max="15" width="22.21875" customWidth="1"/>
-    <col min="16" max="16" width="21.77734375" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" customWidth="1"/>
-    <col min="18" max="18" width="16.88671875" customWidth="1"/>
-    <col min="19" max="19" width="12" customWidth="1"/>
-    <col min="20" max="20" width="17.88671875" customWidth="1"/>
-    <col min="21" max="21" width="26.33203125" customWidth="1"/>
-    <col min="22" max="22" width="13.6640625" customWidth="1"/>
-    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="29" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="16" width="22.21875" customWidth="1"/>
+    <col min="17" max="17" width="21.77734375" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" customWidth="1"/>
+    <col min="19" max="19" width="16.88671875" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="21" max="21" width="17.88671875" customWidth="1"/>
+    <col min="22" max="22" width="26.33203125" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" customWidth="1"/>
+    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -776,63 +765,66 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="P1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="T1" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="U1" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="W1" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -844,13 +836,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
-        <v>48</v>
-      </c>
+      <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -866,8 +858,9 @@
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X2" s="5"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -891,8 +884,9 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -916,8 +910,9 @@
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X4" s="5"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -941,6 +936,7 @@
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -970,25 +966,25 @@
           <x14:formula1>
             <xm:f>options!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6BB6EF60-BAF9-428D-B5C4-8EF858760B90}">
           <x14:formula1>
             <xm:f>options!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>L2:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B14F2C85-AD67-4794-B3E8-7DE4537520AF}">
           <x14:formula1>
             <xm:f>options!$F$2:$F$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>M2:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1D725D8C-87A9-4009-853D-1C43F6BFD1B9}">
           <x14:formula1>
             <xm:f>options!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:Q1048576</xm:sqref>
+          <xm:sqref>R2:R1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1033,7 +1029,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1053,7 +1049,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>14</v>
@@ -1076,7 +1072,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>20</v>
@@ -1099,7 +1095,7 @@
         <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>26</v>
@@ -1114,7 +1110,7 @@
         <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -1127,7 +1123,7 @@
         <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" s="5"/>
     </row>
@@ -1138,7 +1134,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -1150,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8FA5B4-8351-441E-BC93-E5502E84268F}">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1163,26 +1159,27 @@
     <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="22.5546875" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.21875" customWidth="1"/>
-    <col min="13" max="13" width="22.6640625" customWidth="1"/>
-    <col min="14" max="15" width="18" customWidth="1"/>
-    <col min="16" max="16" width="16.77734375" customWidth="1"/>
-    <col min="17" max="17" width="19.44140625" customWidth="1"/>
-    <col min="18" max="18" width="17.109375" customWidth="1"/>
-    <col min="19" max="19" width="19.44140625" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" customWidth="1"/>
-    <col min="21" max="21" width="17.21875" customWidth="1"/>
-    <col min="22" max="22" width="16.77734375" customWidth="1"/>
-    <col min="23" max="23" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.21875" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="15" max="16" width="18" customWidth="1"/>
+    <col min="17" max="17" width="16.77734375" customWidth="1"/>
+    <col min="18" max="18" width="19.44140625" customWidth="1"/>
+    <col min="19" max="19" width="17.109375" customWidth="1"/>
+    <col min="20" max="20" width="19.44140625" customWidth="1"/>
+    <col min="21" max="21" width="19.33203125" customWidth="1"/>
+    <col min="22" max="22" width="17.21875" customWidth="1"/>
+    <col min="23" max="23" width="16.77734375" customWidth="1"/>
+    <col min="24" max="24" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1199,61 +1196,64 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="10" t="s">
-        <v>74</v>
-      </c>
       <c r="P1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="T1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="W1" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="W1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
@@ -1267,60 +1267,63 @@
         <v>11</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="P2" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="S2" s="12" t="s">
+      <c r="T2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="W2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>65</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added origin_destination folders in input and test/input, also added in config files
</commit_message>
<xml_diff>
--- a/input/user_input.xlsx
+++ b/input/user_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC3D29F-9A70-40B8-91EB-B35EFCA63F54}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E1E81F-A774-4BB3-A9B8-38EC15C6DD01}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -1149,7 +1149,7 @@
   <dimension ref="A1:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
klein foutje bij analyses_indirect.py eruit!
</commit_message>
<xml_diff>
--- a/input/user_input.xlsx
+++ b/input/user_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ce\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RA2CE_Sprint\git_race\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64167DC0-07C6-487B-ADAB-B95DAE131A10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6203DA9-0DE9-4ADB-B2F7-43139D28298C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>analysis</t>
   </si>
@@ -173,15 +173,6 @@
     <t>in the unit of the hazard map</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>part_of_DR_roads</t>
-  </si>
-  <si>
-    <t>fid</t>
-  </si>
-  <si>
     <t>snapping_threshold</t>
   </si>
   <si>
@@ -270,6 +261,12 @@
   </si>
   <si>
     <t>name_of_pbf</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>npl_admbnda_adm0_nd_20201117.shp</t>
   </si>
 </sst>
 </file>
@@ -718,37 +715,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="5" max="6" width="21.54296875" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
-    <col min="15" max="16" width="22.21875" customWidth="1"/>
-    <col min="17" max="17" width="21.77734375" customWidth="1"/>
-    <col min="18" max="18" width="20.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" customWidth="1"/>
+    <col min="15" max="16" width="22.1796875" customWidth="1"/>
+    <col min="17" max="17" width="21.81640625" customWidth="1"/>
+    <col min="18" max="18" width="20.6328125" customWidth="1"/>
+    <col min="19" max="19" width="16.90625" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="17.88671875" customWidth="1"/>
-    <col min="22" max="22" width="26.33203125" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" customWidth="1"/>
+    <col min="21" max="21" width="17.90625" customWidth="1"/>
+    <col min="22" max="22" width="26.36328125" customWidth="1"/>
+    <col min="23" max="23" width="13.6328125" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -765,7 +762,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -774,13 +771,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -789,42 +786,42 @@
         <v>8</v>
       </c>
       <c r="N1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" s="14" t="s">
+      <c r="T1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="U1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="V1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="V1" s="15" t="s">
-        <v>61</v>
-      </c>
       <c r="W1" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -833,21 +830,23 @@
         <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -860,7 +859,7 @@
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -886,7 +885,7 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -912,7 +911,7 @@
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1000,16 +999,16 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,10 +1028,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1049,13 +1048,13 @@
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -1072,13 +1071,13 @@
         <v>19</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -1095,13 +1094,13 @@
         <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1110,11 +1109,11 @@
         <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1123,18 +1122,18 @@
         <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -1148,38 +1147,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8FA5B4-8351-441E-BC93-E5502E84268F}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.08984375" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
+    <col min="8" max="8" width="22.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.21875" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="14" max="14" width="22.6328125" customWidth="1"/>
     <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="16.77734375" customWidth="1"/>
-    <col min="18" max="18" width="19.44140625" customWidth="1"/>
-    <col min="19" max="19" width="17.109375" customWidth="1"/>
-    <col min="20" max="20" width="19.44140625" customWidth="1"/>
-    <col min="21" max="21" width="19.33203125" customWidth="1"/>
-    <col min="22" max="22" width="17.21875" customWidth="1"/>
-    <col min="23" max="23" width="16.77734375" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="16.81640625" customWidth="1"/>
+    <col min="18" max="18" width="19.453125" customWidth="1"/>
+    <col min="19" max="19" width="17.08984375" customWidth="1"/>
+    <col min="20" max="20" width="19.453125" customWidth="1"/>
+    <col min="21" max="21" width="19.36328125" customWidth="1"/>
+    <col min="22" max="22" width="17.1796875" customWidth="1"/>
+    <col min="23" max="23" width="16.81640625" customWidth="1"/>
+    <col min="24" max="24" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1196,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>4</v>
@@ -1226,7 +1225,7 @@
         <v>33</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>34</v>
@@ -1238,22 +1237,22 @@
         <v>36</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="X1" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
@@ -1267,13 +1266,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>38</v>
@@ -1296,7 +1295,7 @@
         <v>42</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="12" t="s">
@@ -1306,24 +1305,24 @@
         <v>44</v>
       </c>
       <c r="T2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>62</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
laatste commit inclusief RWS scripts
</commit_message>
<xml_diff>
--- a/input/user_input.xlsx
+++ b/input/user_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ra2ce\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marle\RA2CE_Sprint\git_race\ra2ce\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64167DC0-07C6-487B-ADAB-B95DAE131A10}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6203DA9-0DE9-4ADB-B2F7-43139D28298C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E902DA2C-5FD6-4CAD-9EB8-A76F377A57E5}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>analysis</t>
   </si>
@@ -173,15 +173,6 @@
     <t>in the unit of the hazard map</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>part_of_DR_roads</t>
-  </si>
-  <si>
-    <t>fid</t>
-  </si>
-  <si>
     <t>snapping_threshold</t>
   </si>
   <si>
@@ -270,6 +261,12 @@
   </si>
   <si>
     <t>name_of_pbf</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>npl_admbnda_adm0_nd_20201117.shp</t>
   </si>
 </sst>
 </file>
@@ -718,37 +715,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A046D70D-BBE4-4321-920B-40384B679B05}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="5" max="6" width="21.54296875" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
-    <col min="15" max="16" width="22.21875" customWidth="1"/>
-    <col min="17" max="17" width="21.77734375" customWidth="1"/>
-    <col min="18" max="18" width="20.6640625" customWidth="1"/>
-    <col min="19" max="19" width="16.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.453125" customWidth="1"/>
+    <col min="15" max="16" width="22.1796875" customWidth="1"/>
+    <col min="17" max="17" width="21.81640625" customWidth="1"/>
+    <col min="18" max="18" width="20.6328125" customWidth="1"/>
+    <col min="19" max="19" width="16.90625" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
-    <col min="21" max="21" width="17.88671875" customWidth="1"/>
-    <col min="22" max="22" width="26.33203125" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" customWidth="1"/>
+    <col min="21" max="21" width="17.90625" customWidth="1"/>
+    <col min="22" max="22" width="26.36328125" customWidth="1"/>
+    <col min="23" max="23" width="13.6328125" customWidth="1"/>
     <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -765,7 +762,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -774,13 +771,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -789,42 +786,42 @@
         <v>8</v>
       </c>
       <c r="N1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" s="14" t="s">
+      <c r="T1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="U1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="V1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="V1" s="15" t="s">
-        <v>61</v>
-      </c>
       <c r="W1" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -833,21 +830,23 @@
         <v>10</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="F2" s="5"/>
-      <c r="G2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -860,7 +859,7 @@
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -886,7 +885,7 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -912,7 +911,7 @@
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -1000,16 +999,16 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,10 +1028,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1049,13 +1048,13 @@
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -1072,13 +1071,13 @@
         <v>19</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
@@ -1095,13 +1094,13 @@
         <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1110,11 +1109,11 @@
         <v>27</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1123,18 +1122,18 @@
         <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -1148,38 +1147,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8FA5B4-8351-441E-BC93-E5502E84268F}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.08984375" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" customWidth="1"/>
+    <col min="8" max="8" width="22.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.21875" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="14" max="14" width="22.6328125" customWidth="1"/>
     <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="16.77734375" customWidth="1"/>
-    <col min="18" max="18" width="19.44140625" customWidth="1"/>
-    <col min="19" max="19" width="17.109375" customWidth="1"/>
-    <col min="20" max="20" width="19.44140625" customWidth="1"/>
-    <col min="21" max="21" width="19.33203125" customWidth="1"/>
-    <col min="22" max="22" width="17.21875" customWidth="1"/>
-    <col min="23" max="23" width="16.77734375" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="16.81640625" customWidth="1"/>
+    <col min="18" max="18" width="19.453125" customWidth="1"/>
+    <col min="19" max="19" width="17.08984375" customWidth="1"/>
+    <col min="20" max="20" width="19.453125" customWidth="1"/>
+    <col min="21" max="21" width="19.36328125" customWidth="1"/>
+    <col min="22" max="22" width="17.1796875" customWidth="1"/>
+    <col min="23" max="23" width="16.81640625" customWidth="1"/>
+    <col min="24" max="24" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="87" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>29</v>
       </c>
@@ -1196,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>4</v>
@@ -1226,7 +1225,7 @@
         <v>33</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q1" s="10" t="s">
         <v>34</v>
@@ -1238,22 +1237,22 @@
         <v>36</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="U1" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="V1" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="X1" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
@@ -1267,13 +1266,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>38</v>
@@ -1296,7 +1295,7 @@
         <v>42</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="12"/>
       <c r="R2" s="12" t="s">
@@ -1306,24 +1305,24 @@
         <v>44</v>
       </c>
       <c r="T2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>62</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>